<commit_message>
Test and revise for first publication.
</commit_message>
<xml_diff>
--- a/inst/templates/datatablename_attributes_draft.xlsx
+++ b/inst/templates/datatablename_attributes_draft.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Documents\EDI\data_sets\blank\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Documents\EDI\r\EMLtools\inst\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,18 +19,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>description</t>
+    <t>attributeName</t>
   </si>
   <si>
-    <t>columnName</t>
+    <t>attributeDefinition</t>
   </si>
   <si>
-    <t>unitOrCodeExplanationOrDateFormat</t>
+    <t>class</t>
   </si>
   <si>
-    <t>emptyValueCode</t>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>dateTimeFormatString</t>
+  </si>
+  <si>
+    <t>missingValueCode</t>
+  </si>
+  <si>
+    <t>missingValueCodeExplanation</t>
   </si>
 </sst>
 </file>
@@ -871,21 +880,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -893,6 +908,15 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>